<commit_message>
Fix for xlsb rk values. Unify impl.
</commit_message>
<xml_diff>
--- a/source/Sylvan.Data.Excel.Tests/Data/Numbers.xlsx
+++ b/source/Sylvan.Data.Excel.Tests/Data/Numbers.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\source\Sylvan.Data.Excel\source\Sylvan.Data.Excel.Tests\Data\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\source\Sylvan.Data.Excel\source\Sylvan.Data.Excel.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{339CEC5B-138F-49EB-A8AE-C533F816867C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF86835-D857-49A8-B3CF-8B1C19AD2830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="2220" windowWidth="21600" windowHeight="12735"/>
+    <workbookView xWindow="1305" yWindow="2985" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,11 +366,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,7 +378,7 @@
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>3.3</v>
       </c>
@@ -401,6 +393,9 @@
       </c>
       <c r="E1">
         <v>3.3332999999999999</v>
+      </c>
+      <c r="F1">
+        <v>-9303.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Xlsb rk fix (#40)
* Fix for xlsb rk values. Unify impl.

* bump version.

* Remove temp test
</commit_message>
<xml_diff>
--- a/source/Sylvan.Data.Excel.Tests/Data/Numbers.xlsx
+++ b/source/Sylvan.Data.Excel.Tests/Data/Numbers.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\source\Sylvan.Data.Excel\source\Sylvan.Data.Excel.Tests\Data\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\source\Sylvan.Data.Excel\source\Sylvan.Data.Excel.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{339CEC5B-138F-49EB-A8AE-C533F816867C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF86835-D857-49A8-B3CF-8B1C19AD2830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="2220" windowWidth="21600" windowHeight="12735"/>
+    <workbookView xWindow="1305" yWindow="2985" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,11 +366,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,7 +378,7 @@
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>3.3</v>
       </c>
@@ -401,6 +393,9 @@
       </c>
       <c r="E1">
         <v>3.3332999999999999</v>
+      </c>
+      <c r="F1">
+        <v>-9303.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>